<commit_message>
submit user-answer , check your answer in result page
</commit_message>
<xml_diff>
--- a/back-end/uploads/New Economy TOEIC Test 1/Passages.xlsx
+++ b/back-end/uploads/New Economy TOEIC Test 1/Passages.xlsx
@@ -645,7 +645,7 @@
   <dimension ref="A1:H995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -654,7 +654,7 @@
     <col min="3" max="3" width="30.140625" customWidth="1"/>
     <col min="4" max="4" width="56.28515625" customWidth="1"/>
     <col min="5" max="5" width="39.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>